<commit_message>
All questions now in master
Editing Time!
</commit_message>
<xml_diff>
--- a/OptumBankQuestionsMaster.xlsx
+++ b/OptumBankQuestionsMaster.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16640" yWindow="-19940" windowWidth="18720" windowHeight="18180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14940" yWindow="-21600" windowWidth="34320" windowHeight="20440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="HSA" sheetId="1" r:id="rId1"/>
     <sheet name="FSA" sheetId="2" r:id="rId2"/>
+    <sheet name="HRA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="213">
   <si>
     <t>Question (listed are potential versions of a questioning line posed by a user)</t>
   </si>
@@ -497,10 +498,6 @@
 Can I use my FSA on my kids?</t>
   </si>
   <si>
-    <t>A Eligible dependent care expenses include in-home childcare, payments to licensed day care facilities, before or after school programs, and elder care. You may be reimbursed for dependent care expenses incurred for any individual in your family who’s under age 13 and can be claimed as a dependent on your federal income tax return, or for a spouse or dependent who’s not able to care for him or herself. These expenses must be incurred, regardless of when billed or paid, while you’re working or looking for work. Unlike a health care FSA, you’re only able to receive a reimbursement from a dependent care FSA if sufficient funds have accumulated in your account from payroll deductions.
-It is  a long list, feel free to ask me if a specific thing is covered.</t>
-  </si>
-  <si>
     <t>If my child turns 13 this year, can I use the dependent care account for the whole year?
 When is the last day I can use my FSA on my child?
 Is there an age limit on using my FSA for my kid?</t>
@@ -532,13 +529,793 @@
 "For health care FSAs, your employer determines the minimum and maximum amounts you can set aside in your FSA. However as a result of Health Care Reform beginning January 1, 2013 the maximum contribution amount for the health care FSA will be $2,500. For dependent care FSAs, the annual maximum you can contribute is $5,000, including any amount set aside by a spouse into their dependent care FSA.
 There is a limit of $2,500 for individual FSA's and $5,000 for dependent care FSA's.
 You can only add $2,500 to your own FSA and twice that for dependents."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What happens to the money in a HSA after I turn age 65? 
+What happens to my Health Savings Account after turning 65?
+Tell me about my Health savings account when I'm older/65
+How can I use my Health savings account after turning 65? </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Over the age of 65, you can use your health savings account to pay for non medical expenses, however these will be taxable as income. You will also be able to use the money in your account to pay for any retiree health benefits you might have, or and Medicare related expenses. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up question from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Would you like to hear more about what you can do if you are older than 65? 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You will still be able to use your account for out-of-pocket health expenses tax free. Those enrolled in Medicare can use your account to pay Medicare premiums, deductibles, copays, and coinsurance under any part of Medicare. The one expense that you cannot use your account to pay for is for Medicare supplemental insurance or Medigap policy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I access the funds after I reach age 65?
+How do I get my funds from my health savings account? 
+Can I get my funds from my health savings account? 
+I want to get my funds from my health savings account </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After the age of 65, you can withdraw funds at any time. These funds can be used to pay for medical expenses, and also premiums for Medicare part A or B, Medicare HMO, and employee premiums. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the account beneficiary has attained age 65, are Medicare Part D premiums qualified medical expenses?
+are Medicare Part D premiums medical expenses?
+Can Medicare Part D premiums be used as medical expenses? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you are at least 65 years old, Medicare Part D premiums are qualified as medical expenses. 
+Medicare Part D premiums are qualified as medical expenses if you are the age of 65. 
+Beneficiaries over the age of 65 can use Medicare Part D premiums as medical expenses. The beneficiares spouse and dependents are also qualified. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For the year of 2017, you can contribute $4,400 for individual coverage, and $7,750 for family coverage. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up question from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">There are different contribution rates for 2018 and other benefits for those older than 65. Would you like to hear those? </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2018, you can contribute $4,450 for individual coverage and $7,900 for family coverage. If you are 65, you can make an additional $1,000 catch-up contributions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Support 
+I want customer support
+What is the number for customer support
+How do I get customer support? </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up questions from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Did you transfer your account from Wells Fargo? 
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Get that pen ready? The number for Optum Bank 1-844-326-7967. They are available 24/7. 
+Call Optum Bank at 1-844-326-7967. they are avaiable 24 hours a day. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up question from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Okay. Do you have UHC insurance? </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Get that pen ready! Call 1-800-791-9361. These customer care professionals are available Monday-Friday, 8AM to 8PM. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call 1-866-243-8913. On Monday through Friday, 8.am to 10pm, and Saturday through Sunday 9am to 5:30pm. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are Optum Banks Fees? 
+Tell me about Optum Banks Fees
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up question from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">There are three types of fees: Monthly Maintenance fees, ATM fees, and Outbound Transfer fees. Which would you like to hear about? </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthy Maintenance Fees
+ATM Fees 
+Outbound Transfer Fee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What expenses can I pay for with my health account? 
+</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up Question from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Was it lost, stolen, or are you just in need of an additional card? 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Follow up Question from AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Don't worry, we're here to help. Was it lost or stolen? </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">How much can I contribute to my HSA?
+How much can I put into my HSA?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can I use my Health Savings Account to pay for Long Term Care Insurance?
+I want to use my HSA for Long Term Care 
+How can I pay for Long Term Care Insurance 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, a limited amount Long Term Care insurance can be paid with your HSA. This amount is based on your age. 
+A limited amount of distributions, based on age, can be used for Long Term Care Insurance premiums. 
+Long Term Care insurance premiums qualify as a non penalty medical expense from your HSA, however, the amount of distribution is limted based on your age. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can I use my HSA to pay for health insurance premiums, including Medicare, of a spouse or dependent? 
+Can my HSA pay for my spouse/dependents? 
+Can I use my HSA to pay for health insurance for my spouse / dependents? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only if you are over the age of 65. However, you can only pay for your spouse/dependent if they receive health care coverage through COBRA, or if they are getting unemploymemt compensation. 
+If you are at least 65, you can use your HSA to pay for your spouses/dependents insurance premiums if they are covered by COBRA or have unemployment compensation 
+Those over the age of 65 can pay for their spouses/dependents insurance premiums with HSA. However, they have to be covered by COBRA or unemployment compensation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month by month fee schedules can be found under the "view your account details" tab on the HSA Dashboard after you login. You can also refer to your Optum Bank Welcome Kit or your Employer Open Enrollment materials.
+You are charged $2.50 for each ATM transaction, any any other potential banking fees the atm might have. 
+For every transaction, $2.50 will be charged to your account. The bank's atm might have withdrawl fees. 
+If you want to transfer your HSA to another bank, you will be charged $20.00. 
+$20.00 will be charged to your account if you want to transfer any amount of your HSA to another bank or custodian. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting a new HSA Card
+Can I get a new HSA card? 
+How do I get a new HSA card? 
+</t>
+  </si>
+  <si>
+    <t>My HSA card was lost. 
+My HSA card was stolen. 
+My HSA card is stolen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please call this number: 1-866-234-8913. This is the Optum Bank HSA number. They are available 24 hours a day. The number for Health Advantage Suite of Accounts is 1-800-243-5543. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. 
+I want to order an additional HSA card
+I want another HSA card 
+Can I order a new HSA card? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you want to order additonal cards for either your spouse or dependents, go to Optum Banks website. 
+You can order new HSA cards for your spouse or other dependents if you to to Optum Banks website
+Yes, you can order an additional card. Go to Optum Banks website to order HSA cards for your spouse or other dependents. </t>
+  </si>
+  <si>
+    <t>How can my spouse and I both contribute to an HSA account if we're both covered by HSA-qualified health plans?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Followup Question</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Are the accounts self-only (A4) or family contract (A5)?</t>
+    </r>
+  </si>
+  <si>
+    <t>Self Only Contract</t>
+  </si>
+  <si>
+    <t>Allocate the total contribution between two HSAs as you want as long as you don't contribute more than the statutory maxinmum annual family contribution in total to both HSAs</t>
+  </si>
+  <si>
+    <t>Family Contract</t>
+  </si>
+  <si>
+    <t>You can contribute no more than the statutory maximum annual contribution</t>
+  </si>
+  <si>
+    <t>How do I get a PIN?</t>
+  </si>
+  <si>
+    <t>A new owner can get a PIN when they first activate their debit card. An existing PIN can be changed or found on the customer service number on the back of your card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If I'm covered by an FSA, can I still contribute to an HSA account </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">General Health FSAs are not HSA-eligible but, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Followup Question: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do you have a Limited Purpose (A7) or Post-Deductible FSA (A8)?</t>
+    </r>
+  </si>
+  <si>
+    <t>Limited-Purpose</t>
+  </si>
+  <si>
+    <t>A Limited-Purpose Health FSA reimburses dental and vision expenses and select preventative services which aren't covered completely</t>
+  </si>
+  <si>
+    <t>Post-Deductible</t>
+  </si>
+  <si>
+    <t>A Post-Deductible FSA doesn't begin to pay benefits until the subscriber has met a deductible responsibility equal to the minimum annual deductible for his or her contract type on an HSA-qualified plan</t>
+  </si>
+  <si>
+    <t>Can HSA's be used to pay premiums?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If it's a nonmedical withdrawal, no because they're subject to taxes and penalities. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Followup Question: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is it a medical withdrawal? (A10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>There is no penalty or tax if the money is withdrawn to pay premiums for qualified long term insurance and other cases.</t>
+  </si>
+  <si>
+    <t>What are the different IRS forms?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Followup Question: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What IRS form would you like to learn about? (A12/A13/A14)</t>
+    </r>
+  </si>
+  <si>
+    <t>8899 Form</t>
+  </si>
+  <si>
+    <t>File this form with your income taxes to report year-to-date contributions and distributions from your HSA</t>
+  </si>
+  <si>
+    <t>1099-SA Form</t>
+  </si>
+  <si>
+    <t>This form provides you with the total distributions that were made from your HSA.</t>
+  </si>
+  <si>
+    <t>5498-SA Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This form reports the contributions made to your HSA in that particular tax year. </t>
+  </si>
+  <si>
+    <t>What is an HRA?</t>
+  </si>
+  <si>
+    <t>The Health Reimbursement Arrangements are employer-funded plans that reimburse employees for incurred medical expenses that are not covered by the company's standard insurance plan.</t>
+  </si>
+  <si>
+    <t>What are the benefits of an HRA?
+How does an HRA benefit me?</t>
+  </si>
+  <si>
+    <t>Your employer funds your HRA pre-tax. There are no tax implications since your employer allocates the money. Participating in an HRA is a great way to stretch your healthcare budget. These are just a few of the benefits, would you like to hear more?</t>
+  </si>
+  <si>
+    <t>What types of medical expenses are covered by an HRA?
+What's covered by an HRA?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRA funds must be used for healthcare expenditures only? Approved healthcare expenditures include those identified by your employer as reimbursable from the HRA that are described as Medical Expenses in section 213(d) of the IRS code. More details can be found if you say more. </t>
+  </si>
+  <si>
+    <t>Can I contribute funds to my HRA?
+Can I contribute to my HRA?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No you can not personally contribute. HRAs are only funded by your employer. </t>
+  </si>
+  <si>
+    <t>Can I use an HRA if I have health insurance?</t>
+  </si>
+  <si>
+    <t>Yes. HRA is designed to cover expenses not paid by your health insurance plan</t>
+  </si>
+  <si>
+    <t>What can I pay for with my HRA?
+What does my HRA pay for?</t>
+  </si>
+  <si>
+    <t>HRA funds can be used on eligible expenses determined by your employer</t>
+  </si>
+  <si>
+    <t>How does an HRA work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With an HRA, employers contribute money for each employee to pay for out-of-pocket medical costs. </t>
+  </si>
+  <si>
+    <t>How will I receive the FSA reimbursement?
+How do I get reimbursed for my FSA?</t>
+  </si>
+  <si>
+    <t>After your claim is approved, you will receive a check in the mail or you can sign up for direct deposit.
+If your claim is approved, Optum Bank will send you a check or you can sign up for direct deposit.</t>
+  </si>
+  <si>
+    <t>How often are FSA claims for reimbursement paid?
+How long do FSA claim reimbursements take?</t>
+  </si>
+  <si>
+    <t>Members are typically reimbursed from their FSA within 10 to 14 days. Claims are processed and paid on a weekly basis. Once HealthPartners receives the claim, we take five business days to pay, pend, or deny the claims. 
+Reimbursements typically take 10 to 14 days. Once Healthpartners receives the claim, we take five business days to pay, pend, or deny it.</t>
+  </si>
+  <si>
+    <t>What is acceptable documentation for FSA claims?
+What do I need to make an FSA claim?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There are a number of documents that can and should be submitted for an FSA claim to be accepted. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FOLLOW UP QUESTION FROM AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Would you like to hear some examples?</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes.
+Please provide some examples.</t>
+  </si>
+  <si>
+    <t>Here are a few documents that can be used to make a claim: An explanation of benefits that you received for the medical service; Any receipts that includes the type of service or product provided, the date the expense was incurred, the name of the employee or dependent, the person or organization that provided the service or product, and the amount of the expense; Payment plans should be submitted for regular expenses like orthodontia payment plans; For dependent care expenses, a copy of the bill or signed receipt is acceptable. Make sure your provider has completed the Dependent Care section of the claim form.</t>
+  </si>
+  <si>
+    <t>How do I handle recurring claims on my FSA, like orthodontia?
+Are recurring claims to my FSA handled differently?</t>
+  </si>
+  <si>
+    <t>Recurring claims, like orthodontia payments, can be submitted with supporting payment plan documentation from the service provider. This way, you do not need to send in a claim form for each payment. You will automatically receive monthly allocation reimbursements up to your annual elected amount. However, you do need to submit a new claim each year.</t>
+  </si>
+  <si>
+    <t>How do I keep track of my FSA balance?
+How do I find out how much was reimbursed from my FSA balance?</t>
+  </si>
+  <si>
+    <t>When you request a reimbursement from your FSA, HealthPartners will send you an explanation of benefits statement. The EOB will tell you how much was reimbursed from your FSA.
+Upon requesting a reimbursment, you will receive an explanation of benefits statement that will show your balance.</t>
+  </si>
+  <si>
+    <t>Can I use my Optum Bank FSA even if I am not enrolled in my company’s health plan?
+What if I am not on my company's health plan?</t>
+  </si>
+  <si>
+    <t>You may still be eligible for an FSA provided you meet the requirements. You will have to submit all claims manually via mail or fax. 
+If not enrolled in your company's health plan, you may still meet FSA requirements. All claims will have to be submitted via mail or fax.</t>
+  </si>
+  <si>
+    <t>What happens to the money in the FSA if I leave my employer?
+If I quit my job, what happens to my FSA?</t>
+  </si>
+  <si>
+    <t>If you leave your place of employment during the plan year, you may have a period to submit claims for reimbursement. Services and expenses must have been inucrred before your termination date unless you continue to contribute to your FSA account through COBRA.</t>
+  </si>
+  <si>
+    <t>If my FSA plan offers a grace period, how does that affect my eligibility for an HSA?
+Can I have an HSA if I am in my FSA plan grace period?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legislation regarding HSA/FSA coordination allows you to enroll in an HSA if: either there is no money left in the FSA at the end of the plan year, or you make a one-time rollover from the FSA to the HSA, as allowed by your employer. </t>
+  </si>
+  <si>
+    <t>Are there any special considerations for spouses working at the same company?
+What if my spouse also works at my company?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In order for the automatic claims submission to work, the policy holder on the Optum Bank medical/dental plan and the participant on the FSA need to be the same person. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">How does participation in my employer’s dependent care FSA affect my ability to claim the dependent care tax credit on my federal income tax returns?
+Will a dependent care FSA affect my federal income tax returns?
+</t>
+  </si>
+  <si>
+    <t>You cannot claim a dependent care tax credit for amounts received under an employer’s FSA plan. You may wish to consult with a tax advisor to determine whether the FSA plan or the dependent care tax credit is more beneficial in your individual case. Generally, the higher your income, the more beneficial it is to participate in the dependent care FSA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I contribute more to my HSA? 
+What ways can I add money to my HSA?
+</t>
+  </si>
+  <si>
+    <t>HSA contributions can be through payroll deductions, or by going online and making a contribution from your personal account.
+You can contribute to your HSA either through contributions made via payroll deductions by your employer, or by logging on to Optumbank.com and making a contribution from your personal checking or savings account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can I transfer Optum Bank HSA money to my personal bank account?
+</t>
+  </si>
+  <si>
+    <t>Yes, you can transfer funds via direct deposit directly into your account.
+Yes, through direct deposit.</t>
+  </si>
+  <si>
+    <t>Can I use Quicken with Optum Bank?</t>
+  </si>
+  <si>
+    <t>Yes, account holders will be able to download transactions into Quicken from their Optum Bank HSA.
+Yes, you can download HSA transactions to your Quicken account.</t>
+  </si>
+  <si>
+    <t>How will Optum Bank handle accounts that reach the annual maximum?
+What if I reach the annual maximum on my account?</t>
+  </si>
+  <si>
+    <t>Communication is sent to account holders when accounts are close to reaching the annual maximum. 
+Optum Bank will alert you when you are nearing the annual maximum.</t>
+  </si>
+  <si>
+    <t>Is the Optum Bank investment sweep a one-way sweep from the cash account to the investment?
+How does the Optum Bank investment sweep work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Optum Bank investment sweep is a one-way sweep from the Optum Bank HSA to the investment account.</t>
+  </si>
+  <si>
+    <t>Does the investment balance show online with a breakdown of the dollars in each fund?
+How is my investment balance shown?</t>
+  </si>
+  <si>
+    <t>The Optum Bank website shows both the aggregate balance and the balance by fund.
+Go to OptumBank.com, where you can see both your aggregate balance and a breakdown of balance by fund.</t>
+  </si>
+  <si>
+    <t>How is the Optum Bank investment sweep activated and deactivated?
+How do I activate the Optum Bank investment sweep?
+How do I deactivate the Optum Bank investment sweep?</t>
+  </si>
+  <si>
+    <t>Activating or deactivating the investment sweep is available online or by calling the call center, but the account must be registered prior to the call.
+To activate or deactivate your account, log in online or call us. Note that the account must be registered prior to telephone activation or deactivation.</t>
+  </si>
+  <si>
+    <t>Can the Optum Bank HSA be used with mobile wallets such as Apple Pay, Android Pay, Samsung Pay, and Google Wallet?
+Can I use a mobile payment app with Optum Bank HSA?</t>
+  </si>
+  <si>
+    <t>Optum Bank does not currently offer connectivity with mobile wallets, but will offer this in a future enhancement. If you currently have a tokenized card, this functionality will not be migrated.</t>
+  </si>
+  <si>
+    <t>How frequently will Optum Bank statements be generated?
+When will I get my bank statements?</t>
+  </si>
+  <si>
+    <t>Optum Bank statements are issued on a monthly basis.
+Bank statements are sent out monthly.</t>
+  </si>
+  <si>
+    <t>How can I use my HSA to pay for qualified medical expenses?
+How do I pay for my medical expenses?</t>
+  </si>
+  <si>
+    <t>The easiest way to pay your medical expenses is by using your Optum Bank Health Savings Account Debit Mastercard. Other alternatives include paying bills online by logging into your account and sending payments directly to your health care providers, or paying out of pocket and reimbursing yourself by requesting an electronic reimbursement online.
+You can pay your expenses by using your Optum Bank HSA debit card, paying your bills online and sending payments directly to your healthcare providers, or by paying out of pocket and requesting an electronic reimbursement online.</t>
+  </si>
+  <si>
+    <t>How are Optum Bank statements generated: paper, online, or both? 
+How do I view my bank statements?
+How long are bank statements stored online to be available for download?</t>
+  </si>
+  <si>
+    <t>Statements are available both online and on paper. Statements remain online for 36 months, whereas paper statements can be requested at any time.
+Online statements can be accessed on our website and remain online for 36 months. Paper statements can be requested at any time.</t>
+  </si>
+  <si>
+    <t>Where can I obtain a copy of my tax forms?
+How do I see tax forms?</t>
+  </si>
+  <si>
+    <t>Your forms can be found by logging into your online account and viewing your statements.
+Log into your account on OptumBank.com to view your tax forms.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How can I order an additional debit card or get a PIN?
+Can I get more than one debit card?
+</t>
+  </si>
+  <si>
+    <t>You can order additional cards online. You will be able to choose a PIN when you first activate your debit card.
+Additional cards can be ordered online. You can choose a new PIN upon card activation.</t>
+  </si>
+  <si>
+    <t>How do I start using my HSA?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Follow our new account holder checklist to get off to a good start.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FOLLOW UP QUESTION FROM AI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Would you like to hear more about this?</t>
+    </r>
+  </si>
+  <si>
+    <t>Yes.
+Yes, tell me about the new account holder checklist.</t>
+  </si>
+  <si>
+    <t>Using our website, navigate to the new account holder checklist in the customer-support section. This checklist will guide you through registering for online access to your account and starting to make contributions.</t>
+  </si>
+  <si>
+    <t>I'm thinking about opening an HSA, am I eligible?
+Am I eligible to open an HSA?</t>
+  </si>
+  <si>
+    <t>The main requirement for opening an HSA is having a high-deductible health plan that meets IRS guidelines.
+In order to be eligible for an HSA, you must have a high-deductible health plan that meets IRS guidelines.</t>
+  </si>
+  <si>
+    <t>Eligible dependent care expenses include in-home childcare, payments to licensed day care facilities, before or after school programs, and elder care. You may be reimbursed for dependent care expenses incurred for any individual in your family who’s under age 13 and can be claimed as a dependent on your federal income tax return, or for a spouse or dependent who’s not able to care for him or herself. These expenses must be incurred, regardless of when billed or paid, while you’re working or looking for work. Unlike a health care FSA, you’re only able to receive a reimbursement from a dependent care FSA if sufficient funds have accumulated in your account from payroll deductions.
+It is  a long list, feel free to ask me if a specific thing is covered.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -603,7 +1380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,14 +1389,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB7DEE8"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -635,7 +1405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -645,169 +1415,188 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="13" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="40">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="13" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1136,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1152,269 +1941,875 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="13" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" ht="60">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="15" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="45">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" ht="90">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="60">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="13" t="s">
         <v>20</v>
       </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="60">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="16" t="s">
         <v>24</v>
       </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="13" t="s">
         <v>26</v>
       </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="60">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" ht="45">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="16" t="s">
         <v>30</v>
       </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5" ht="75">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="16" t="s">
         <v>32</v>
       </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="13" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="45">
-      <c r="A17" s="7" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" ht="45">
+      <c r="A17" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="16" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="75">
-      <c r="A18" s="9" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" ht="75">
+      <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="75">
-      <c r="A19" s="10" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" ht="75">
+      <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="75">
-      <c r="A20" s="9" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" ht="75">
+      <c r="A20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="120">
-      <c r="A21" s="10" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="120">
+      <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="105">
-      <c r="A22" s="9" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="105">
+      <c r="A22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="90">
-      <c r="A23" s="11" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" ht="90">
+      <c r="A23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="105">
-      <c r="A24" s="9" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" ht="105">
+      <c r="A24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="150">
-      <c r="A25" s="11" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" ht="150">
+      <c r="A25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="75">
-      <c r="A26" s="9" t="s">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" ht="75">
+      <c r="A26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="75">
-      <c r="A27" s="11" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" ht="75">
+      <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="90">
-      <c r="A28" s="12" t="s">
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" ht="90">
+      <c r="A28" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="75">
-      <c r="A29" s="3" t="s">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" ht="75">
+      <c r="A29" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="90">
-      <c r="A30" s="13" t="s">
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="1:5" ht="90">
+      <c r="A30" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" ht="120">
+      <c r="A31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32" spans="1:5" ht="60">
+      <c r="A32" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" ht="75">
+      <c r="A33" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" ht="120">
+      <c r="A34" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" ht="90">
+      <c r="A35" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="135">
+      <c r="A36" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" ht="60">
+      <c r="A37" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" ht="60">
+      <c r="A39" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+    </row>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" spans="1:5" ht="30">
+      <c r="A43" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+    </row>
+    <row r="44" spans="1:5" ht="45">
+      <c r="A44" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+    </row>
+    <row r="45" spans="1:5" ht="210">
+      <c r="A45" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+    </row>
+    <row r="46" spans="1:5" ht="45">
+      <c r="A46" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+    </row>
+    <row r="47" spans="1:5" ht="75">
+      <c r="A47" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+    </row>
+    <row r="48" spans="1:5" ht="45">
+      <c r="A48" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+    </row>
+    <row r="49" spans="1:5" ht="120">
+      <c r="A49" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+    </row>
+    <row r="50" spans="1:5" ht="30">
+      <c r="A50" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+    </row>
+    <row r="51" spans="1:5" ht="45">
+      <c r="A51" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+    </row>
+    <row r="53" spans="1:5" ht="30">
+      <c r="A53" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+    </row>
+    <row r="55" spans="1:5" ht="30">
+      <c r="A55" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+    </row>
+    <row r="56" spans="1:5" ht="45">
+      <c r="A56" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:5" ht="30">
+      <c r="A58" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+    </row>
+    <row r="59" spans="1:5" ht="30">
+      <c r="A59" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+    </row>
+    <row r="64" spans="1:5" ht="75">
+      <c r="A64" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" spans="1:5" ht="45">
+      <c r="A65" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+    </row>
+    <row r="66" spans="1:5" ht="45">
+      <c r="A66" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+    </row>
+    <row r="67" spans="1:5" ht="45">
+      <c r="A67" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+    </row>
+    <row r="68" spans="1:5" ht="45">
+      <c r="A68" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+    </row>
+    <row r="69" spans="1:5" ht="45">
+      <c r="A69" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" spans="1:5" ht="60">
+      <c r="A70" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+    </row>
+    <row r="71" spans="1:5" ht="45">
+      <c r="A71" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+    </row>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+    </row>
+    <row r="73" spans="1:5" ht="105">
+      <c r="A73" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+    </row>
+    <row r="74" spans="1:5" ht="75">
+      <c r="A74" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+    </row>
+    <row r="75" spans="1:5" ht="30">
+      <c r="A75" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+    </row>
+    <row r="76" spans="1:5" ht="45">
+      <c r="A76" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+    </row>
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+    </row>
+    <row r="78" spans="1:5" ht="45">
+      <c r="A78" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B78" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+    </row>
+    <row r="79" spans="1:5" ht="60">
+      <c r="A79" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1429,10 +2824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1442,116 +2837,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="27" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="27" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="150">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="8" spans="1:5" ht="150">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="28" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="90">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="10" spans="1:5" ht="135">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="28" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="150">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60">
+      <c r="A12" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="18" t="s">
+      <c r="B12" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="19" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="90">
+      <c r="A13" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="90">
-      <c r="A13" s="20" t="s">
+      <c r="B13" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>82</v>
+    </row>
+    <row r="14" spans="1:5" ht="60">
+      <c r="A14" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="75">
+      <c r="A15" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45">
+      <c r="A16" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="120">
+      <c r="A17" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="75">
+      <c r="A18" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="75">
+      <c r="A19" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="60">
+      <c r="A20" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60">
+      <c r="A21" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60">
+      <c r="A22" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="45">
+      <c r="A23" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="90">
+      <c r="A24" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1563,4 +3046,84 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="58.5" customWidth="1"/>
+    <col min="2" max="2" width="75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="45">
+      <c r="A1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45">
+      <c r="A2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60">
+      <c r="A3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>